<commit_message>
Updates for Order Receipt page + selenium tests
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
+++ b/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1940" yWindow="60" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="172">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -433,9 +433,6 @@
     <t>To test that the order receipt contains the items placed on order</t>
   </si>
   <si>
-    <t>OrderPage_TCase_1</t>
-  </si>
-  <si>
     <t>Adam Hale</t>
   </si>
   <si>
@@ -466,21 +463,6 @@
     <t>OrderPage_TConn_6</t>
   </si>
   <si>
-    <t>OrderPage_TCase_2</t>
-  </si>
-  <si>
-    <t>OrderPage_TCase_3</t>
-  </si>
-  <si>
-    <t>OrderPage_TCase_4</t>
-  </si>
-  <si>
-    <t>OrderPage_TCase_6</t>
-  </si>
-  <si>
-    <t>OrderPage_TCase_5</t>
-  </si>
-  <si>
     <t>To test that the order receipt contains the items placed on order, specifically looking to see if it records the additional extras</t>
   </si>
   <si>
@@ -574,24 +556,15 @@
     <t>The Order receipt should include the confirmed date and time for collection having selected the later option for collection but choosing a time that has already passed</t>
   </si>
   <si>
-    <t>OrderPage_TCase_7</t>
-  </si>
-  <si>
     <t>Having added an order to the basket with extras and confirmed the collection time as later and selecting a date that has passed, that it does not progress to the order receipt</t>
   </si>
   <si>
     <t xml:space="preserve">Order receipt will not be generated until valid date is input </t>
   </si>
   <si>
-    <t>OrderPage_TCase_8</t>
-  </si>
-  <si>
     <t>Having added an order to the basket with extras and confirmed the collection time as later and selecting a time that has passed, that it does not progress to the order receipt</t>
   </si>
   <si>
-    <t>OrderPage_TCase_9</t>
-  </si>
-  <si>
     <t>The Order receipt should include a unique order reference different to the test before</t>
   </si>
   <si>
@@ -643,9 +616,6 @@
     <t>Meat Extravaganza with peppers</t>
   </si>
   <si>
-    <t>OrderPage_TCase_10</t>
-  </si>
-  <si>
     <t>This is the same order reference as the prevois test case thererfore it is not unique, it is not critical or high as it will not lead to system crash or failure, it will just cause significant difficulties on collection</t>
   </si>
   <si>
@@ -662,6 +632,126 @@
   </si>
   <si>
     <t>OrderPage_3</t>
+  </si>
+  <si>
+    <t>Having changed password, does the system still work and process the order providing a receipt</t>
+  </si>
+  <si>
+    <t>Changed password and when through ordering process again to make sure that an order receipt is generated</t>
+  </si>
+  <si>
+    <t>Deluxe with olives</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_11</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>The Order receipt should be generated when a user changes their password and places and order</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having changed the users password and placing an order, the order receipt will still be generated </t>
+  </si>
+  <si>
+    <t>Order receipt will be successfully displayed with the correct order details and the unique order reference</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_1</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_2</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_3</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_4</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_5</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_6</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_7</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_8</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_9</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_10</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_11</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_1</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_2</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_3</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_4</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_5</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_6</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_7</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_8</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_9</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_10</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_11</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_3</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_4</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_5</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_6</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_7</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_8</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_9</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_10</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_11</t>
   </si>
 </sst>
 </file>
@@ -874,8 +964,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="203">
+  <cellStyleXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1175,7 +1277,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="203">
+  <cellStyles count="215">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1277,6 +1379,12 @@
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1378,6 +1486,12 @@
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1435,6 +1549,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1444,6 +1559,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1453,6 +1569,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1491,7 +1608,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.0</c:v>
@@ -1517,6 +1634,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1613,11 +1731,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2090090136"/>
-        <c:axId val="2090087176"/>
+        <c:axId val="2071990488"/>
+        <c:axId val="2071987528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2090090136"/>
+        <c:axId val="2071990488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090087176"/>
+        <c:crossAx val="2071987528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1634,7 +1752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090087176"/>
+        <c:axId val="2071987528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090090136"/>
+        <c:crossAx val="2071990488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2059,7 +2177,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2085,7 +2203,7 @@
     </row>
     <row r="2" spans="1:9" ht="35.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>58</v>
@@ -2102,7 +2220,7 @@
     </row>
     <row r="3" spans="1:9" ht="35.5" customHeight="1">
       <c r="A3" s="32" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>60</v>
@@ -2117,7 +2235,7 @@
     </row>
     <row r="4" spans="1:9" ht="28">
       <c r="A4" s="32" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>61</v>
@@ -2134,7 +2252,7 @@
     </row>
     <row r="5" spans="1:9" ht="23">
       <c r="A5" s="32" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>62</v>
@@ -2151,10 +2269,10 @@
     </row>
     <row r="6" spans="1:9" ht="28">
       <c r="A6" s="32" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>59</v>
@@ -2168,10 +2286,10 @@
     </row>
     <row r="7" spans="1:9" ht="28">
       <c r="A7" s="32" t="s">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>59</v>
@@ -2185,10 +2303,10 @@
     </row>
     <row r="8" spans="1:9" ht="42">
       <c r="A8" s="32" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>59</v>
@@ -2202,10 +2320,10 @@
     </row>
     <row r="9" spans="1:9" ht="42">
       <c r="A9" s="32" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>59</v>
@@ -2216,7 +2334,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="32" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>63</v>
@@ -2230,10 +2348,10 @@
     </row>
     <row r="11" spans="1:9" ht="28">
       <c r="A11" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>109</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>118</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>59</v>
@@ -2242,11 +2360,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+    <row r="12" spans="1:9" ht="28">
+      <c r="A12" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="D13" s="1"/>
@@ -2283,8 +2409,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2356,19 +2482,19 @@
     </row>
     <row r="2" spans="1:26" ht="52">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -2380,7 +2506,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -2395,19 +2521,19 @@
     </row>
     <row r="3" spans="1:26" ht="65">
       <c r="A3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>27</v>
@@ -2419,7 +2545,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
@@ -2434,19 +2560,19 @@
     </row>
     <row r="4" spans="1:26" ht="52">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>154</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>27</v>
@@ -2458,10 +2584,10 @@
         <v>25</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>33</v>
@@ -2473,10 +2599,10 @@
         <v>42074</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Z4" s="5" t="s">
@@ -2485,19 +2611,19 @@
     </row>
     <row r="5" spans="1:26" ht="52">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>27</v>
@@ -2509,7 +2635,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="4"/>
@@ -2521,19 +2647,19 @@
     </row>
     <row r="6" spans="1:26" ht="65">
       <c r="A6" s="1" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -2545,10 +2671,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>33</v>
@@ -2560,28 +2686,28 @@
         <v>42074</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="65">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -2593,7 +2719,7 @@
         <v>24</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="4"/>
@@ -2608,19 +2734,19 @@
     </row>
     <row r="8" spans="1:26" ht="52">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
@@ -2632,7 +2758,7 @@
         <v>24</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="4"/>
@@ -2646,24 +2772,24 @@
       </c>
       <c r="U8" s="31">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="52">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
@@ -2675,7 +2801,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="4"/>
@@ -2694,19 +2820,19 @@
     </row>
     <row r="10" spans="1:26" ht="52">
       <c r="A10" s="1" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>6</v>
@@ -2718,7 +2844,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="4"/>
@@ -2735,21 +2861,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="65">
+    <row r="11" spans="1:26" ht="76" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>6</v>
@@ -2761,10 +2887,10 @@
         <v>25</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>33</v>
@@ -2776,20 +2902,44 @@
         <v>42074</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:26" ht="65">
+      <c r="A12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="34">
+        <v>42086</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="1:26">
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -4974,14 +5124,14 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="5" width="24.1640625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
@@ -5017,19 +5167,19 @@
     </row>
     <row r="2" spans="1:13" ht="42">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="27" t="s">
@@ -5043,19 +5193,19 @@
     </row>
     <row r="3" spans="1:13" ht="56">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -5068,19 +5218,19 @@
     </row>
     <row r="4" spans="1:13" ht="56">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -5093,19 +5243,19 @@
     </row>
     <row r="5" spans="1:13" ht="42">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -5118,19 +5268,19 @@
     </row>
     <row r="6" spans="1:13" ht="42">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -5143,19 +5293,19 @@
     </row>
     <row r="7" spans="1:13" ht="56">
       <c r="A7" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -5168,19 +5318,19 @@
     </row>
     <row r="8" spans="1:13" ht="56">
       <c r="A8" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>167</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -5193,19 +5343,19 @@
     </row>
     <row r="9" spans="1:13" ht="56">
       <c r="A9" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -5218,19 +5368,19 @@
     </row>
     <row r="10" spans="1:13" ht="56">
       <c r="A10" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -5243,19 +5393,19 @@
     </row>
     <row r="11" spans="1:13" ht="56">
       <c r="A11" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -5266,12 +5416,22 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="12" spans="1:13" ht="71" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -5489,12 +5649,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5608,7 +5762,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5617,16 +5771,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5642,10 +5793,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test updates to order receipt page
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
+++ b/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="60" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="15080" windowHeight="15140" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="337">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -550,9 +550,6 @@
     <t>OrderPage_TConn_10</t>
   </si>
   <si>
-    <t>The Order receipt should include the confirmed date and time for collection having selected the later option for collection but choosing a date that has already passed</t>
-  </si>
-  <si>
     <t>The Order receipt should include the confirmed date and time for collection having selected the later option for collection but choosing a time that has already passed</t>
   </si>
   <si>
@@ -646,9 +643,6 @@
     <t>OrderPage_TConn_11</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>The Order receipt should be generated when a user changes their password and places and order</t>
   </si>
   <si>
@@ -752,6 +746,508 @@
   </si>
   <si>
     <t>OrderReceipt_TConn_11</t>
+  </si>
+  <si>
+    <t>The Order receipt should not be accessed having confirmed date and time for collection, selecting the later option for collection but choosing a date that has already passed</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_12</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_13</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_14</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_15</t>
+  </si>
+  <si>
+    <t>The Order receipt page should have the company logo in the header of the web page</t>
+  </si>
+  <si>
+    <t>The Order receipt page should have a copyright and site version in the footer</t>
+  </si>
+  <si>
+    <t>The Order receipt page should have a title for the page</t>
+  </si>
+  <si>
+    <t>The Order receipt page should have navigation accessible on the page</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>4.1.7</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_12</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_13</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_14</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_15</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_12</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_13</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_14</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_15</t>
+  </si>
+  <si>
+    <t>When on the Order Receipt page, the company logo should be in the header of the page</t>
+  </si>
+  <si>
+    <t>Having ordered a pizza and confirmed collection</t>
+  </si>
+  <si>
+    <t>Cheese Pizza</t>
+  </si>
+  <si>
+    <t>When on the Order Receipt page, the company Copyright and site version should be in the footer of the page</t>
+  </si>
+  <si>
+    <t>When on the Order Receipt page, there will be a title telling the user what page they are on</t>
+  </si>
+  <si>
+    <t>When on the Order Receipt page, there will be  common navagation method for users to use</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_12</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_13</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_14</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_15</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_12</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_13</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_14</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_15</t>
+  </si>
+  <si>
+    <t>Having added a plain cheese pizza to the basket and confirmed collection, the user should see the company logo in the header of the page</t>
+  </si>
+  <si>
+    <t>There will be the company logo within the header of the page</t>
+  </si>
+  <si>
+    <t>exploratory</t>
+  </si>
+  <si>
+    <t>Having added a plain cheese pizza to the basket and confirmed collection, the user should see the company copyright and site version in the footer of the page</t>
+  </si>
+  <si>
+    <t>There will be the company copyright and site version in the footer of the page</t>
+  </si>
+  <si>
+    <t>Having added a plain cheese pizza to the basket and confirmed collection, the user should see the title of the page they are on</t>
+  </si>
+  <si>
+    <t>There will be a title for the Order Receipt page</t>
+  </si>
+  <si>
+    <t>There will be common navigation on the page</t>
+  </si>
+  <si>
+    <t>Having added a plain cheese pizza to the basket and confirmed collection, the user should see common navagation on the page</t>
+  </si>
+  <si>
+    <t>OrderPage_Tcon_13</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no copyright in the footer, also need to clarify if "2015 - QUB CSC3056 CSC7056" is valid for site version
+</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_16</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_17</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_18</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_19</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_16</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_17</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_18</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_19</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_16</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_17</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_18</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_19</t>
+  </si>
+  <si>
+    <t>Test the the navigation for "Home" works from the Order Receipt page</t>
+  </si>
+  <si>
+    <t>Test the the navigation for "Order" works from the Order Receipt page</t>
+  </si>
+  <si>
+    <t>Test the the navigation for "About" works from the Order Receipt page</t>
+  </si>
+  <si>
+    <t>Test the the navigation for "Contact" works from the Order Receipt page</t>
+  </si>
+  <si>
+    <t>User will be directed to the Home page</t>
+  </si>
+  <si>
+    <t>User will be directed to the Order page</t>
+  </si>
+  <si>
+    <t>User will be directed to the About page</t>
+  </si>
+  <si>
+    <t>User will be directed to the Contact page</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_16</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_17</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_18</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_19</t>
+  </si>
+  <si>
+    <t>Test that clicking on the navigation for Order will direct user to Order page</t>
+  </si>
+  <si>
+    <t>Test that clicking on the navigation for Home will direct user to Home page</t>
+  </si>
+  <si>
+    <t>Test that clicking on the navigation for About will direct user to About page</t>
+  </si>
+  <si>
+    <t>Test that clicking on the navigation for Contact will direct user to Contact page</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_16</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_17</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_18</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_19</t>
+  </si>
+  <si>
+    <t>4.1.8</t>
+  </si>
+  <si>
+    <t>Having clicked on the Home navigation while on the Order Receipt page, the user will be directed to the Home page</t>
+  </si>
+  <si>
+    <t>Having clicked on the Contact navigation while on the Order Receipt page, the user will be directed to the Contact page</t>
+  </si>
+  <si>
+    <t>Having clicked on the About navigation while on the Order Receipt page, the user will be directed to the About page</t>
+  </si>
+  <si>
+    <t>Having clicked on the Order navigation while on the Order Receipt page, the user will be directed to the Order page</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_20</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_21</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_22</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_23</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_24</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_25</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_26</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_27</t>
+  </si>
+  <si>
+    <t>From the Order Receipt page, a user that is logged in can navigate to the reset password page</t>
+  </si>
+  <si>
+    <t>Users that are logged in should be able to log off from the Order Receipt page</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_20</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_21</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_22</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_23</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_24</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_25</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_26</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_27</t>
+  </si>
+  <si>
+    <t>Any user that is not registered should not be able to access the Order Receipt page</t>
+  </si>
+  <si>
+    <t>Test the Order Receipt page on … mobile device</t>
+  </si>
+  <si>
+    <t>Test the Order Receipt page on Google Chrome browser, version 36</t>
+  </si>
+  <si>
+    <t>Test the Order Receipt page on Internet Explorer 11</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_20</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_21</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_22</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_23</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_24</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_25</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_26</t>
+  </si>
+  <si>
+    <t>4.1.10</t>
+  </si>
+  <si>
+    <t>To ensure all logged users can navigate to the reset password page</t>
+  </si>
+  <si>
+    <t>To ensure that logged users can log off from the Order receipt page</t>
+  </si>
+  <si>
+    <t>To check the Schedule web page works on different browser types</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_27</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_28</t>
+  </si>
+  <si>
+    <t>OrderReceip_TCase_29</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_28</t>
+  </si>
+  <si>
+    <t>OrderPage_TConn_29</t>
+  </si>
+  <si>
+    <t>To check the Order Receipt page works on the Amazon Kindle Fire 7 inch mobile device</t>
+  </si>
+  <si>
+    <t>To check the Order Receipt page worls on the iPad 4 mobile device</t>
+  </si>
+  <si>
+    <t>To check the Order Receipt page works on the iPhone 6 mobile device</t>
+  </si>
+  <si>
+    <t>To check the Order Receipt page works on the Google Nexus 10 mobile device</t>
+  </si>
+  <si>
+    <t>To check the Order Receipt page works on the Samsung Galaxy S4 mobile device</t>
+  </si>
+  <si>
+    <t>To check that unregistered users or not logged in users can't access the Order Receipt page</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_28</t>
+  </si>
+  <si>
+    <t>OrderReceip_TConn_29</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_20</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_21</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_22</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_23</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_24</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_25</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_26</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_27</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_28</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_29</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_20</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_21</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_22</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_23</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_24</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_25</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_26</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_27</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_28</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_29</t>
+  </si>
+  <si>
+    <t>The system should prevent unregistered users accessing the Schedule Order page</t>
+  </si>
+  <si>
+    <t>Test Order Receipt page on a iPhone 6 mobile device</t>
+  </si>
+  <si>
+    <t>Test Order Receipt page on a Chrome Web Browser, version 36</t>
+  </si>
+  <si>
+    <t>Test OrderReceipt  page on  a version of Internet Explorer 11</t>
+  </si>
+  <si>
+    <t>Test Order Receipt page on a iPad 4 mobile device</t>
+  </si>
+  <si>
+    <t>Test Order Receipt page on a Amazon Kindle Fire 7 inch mobile device</t>
+  </si>
+  <si>
+    <t>Test Order Receipt page on a Google Nexus 10 mobile device</t>
+  </si>
+  <si>
+    <t>Test Order Receipt page on a Samsung Galaxy S4 mobile device</t>
+  </si>
+  <si>
+    <t>Order Receipt page opens as intended</t>
+  </si>
+  <si>
+    <t>Unregistered users are ristricted and are not allowed to view the Order Receipt page</t>
+  </si>
+  <si>
+    <t>User is able to log of from Order Receipt page</t>
+  </si>
+  <si>
+    <t>User is able to get to the reset password page and reset password from Order Receipt page</t>
+  </si>
+  <si>
+    <t>From the Order Receipt page, a logged user can navigate to the reset password page</t>
+  </si>
+  <si>
+    <t>A logged user should be able to log off from the Order Receipt page</t>
   </si>
 </sst>
 </file>
@@ -964,7 +1460,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="309">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1180,8 +1676,102 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1276,8 +1866,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="309">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1385,6 +1979,53 @@
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1492,6 +2133,53 @@
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1608,13 +2296,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,10 +2392,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1731,11 +2419,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2071990488"/>
-        <c:axId val="2071987528"/>
+        <c:axId val="2107205560"/>
+        <c:axId val="2107208504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2071990488"/>
+        <c:axId val="2107205560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +2432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2071987528"/>
+        <c:crossAx val="2107208504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1752,7 +2440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2071987528"/>
+        <c:axId val="2107208504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +2451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2071990488"/>
+        <c:crossAx val="2107205560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2174,10 +2862,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF023FAE"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2203,7 +2891,7 @@
     </row>
     <row r="2" spans="1:9" ht="35.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>58</v>
@@ -2220,7 +2908,7 @@
     </row>
     <row r="3" spans="1:9" ht="35.5" customHeight="1">
       <c r="A3" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>60</v>
@@ -2235,7 +2923,7 @@
     </row>
     <row r="4" spans="1:9" ht="28">
       <c r="A4" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>61</v>
@@ -2252,7 +2940,7 @@
     </row>
     <row r="5" spans="1:9" ht="23">
       <c r="A5" s="32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>62</v>
@@ -2269,7 +2957,7 @@
     </row>
     <row r="6" spans="1:9" ht="28">
       <c r="A6" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>93</v>
@@ -2286,7 +2974,7 @@
     </row>
     <row r="7" spans="1:9" ht="28">
       <c r="A7" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>96</v>
@@ -2303,10 +2991,10 @@
     </row>
     <row r="8" spans="1:9" ht="42">
       <c r="A8" s="32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>59</v>
@@ -2320,10 +3008,10 @@
     </row>
     <row r="9" spans="1:9" ht="42">
       <c r="A9" s="32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>59</v>
@@ -2334,7 +3022,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>63</v>
@@ -2348,10 +3036,10 @@
     </row>
     <row r="11" spans="1:9" ht="28">
       <c r="A11" s="32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>59</v>
@@ -2362,10 +3050,10 @@
     </row>
     <row r="12" spans="1:9" ht="28">
       <c r="A12" s="32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>59</v>
@@ -2374,11 +3062,257 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="D14" s="1"/>
+    <row r="13" spans="1:9" ht="28">
+      <c r="A13" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28">
+      <c r="A14" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28">
+      <c r="A16" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28">
+      <c r="A17" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28">
+      <c r="A18" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28">
+      <c r="A19" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28">
+      <c r="A20" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28">
+      <c r="A21" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28">
+      <c r="A23" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28">
+      <c r="A24" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28">
+      <c r="A25" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28">
+      <c r="A26" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28">
+      <c r="A27" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28">
+      <c r="A28" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28">
+      <c r="A29" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28">
+      <c r="A30" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2391,7 +3325,7 @@
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D14</xm:sqref>
+          <xm:sqref>D2:D12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2409,8 +3343,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="E14" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2482,7 +3416,7 @@
     </row>
     <row r="2" spans="1:26" ht="52">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>64</v>
@@ -2521,7 +3455,7 @@
     </row>
     <row r="3" spans="1:26" ht="65">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>75</v>
@@ -2560,7 +3494,7 @@
     </row>
     <row r="4" spans="1:26" ht="52">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>85</v>
@@ -2587,7 +3521,7 @@
         <v>65</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>33</v>
@@ -2611,7 +3545,7 @@
     </row>
     <row r="5" spans="1:26" ht="52">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>89</v>
@@ -2647,7 +3581,7 @@
     </row>
     <row r="6" spans="1:26" ht="65">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>92</v>
@@ -2674,7 +3608,7 @@
         <v>65</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>33</v>
@@ -2695,7 +3629,7 @@
     </row>
     <row r="7" spans="1:26" ht="65">
       <c r="A7" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>97</v>
@@ -2734,10 +3668,10 @@
     </row>
     <row r="8" spans="1:26" ht="52">
       <c r="A8" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>76</v>
@@ -2772,15 +3706,15 @@
       </c>
       <c r="U8" s="31">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="52">
       <c r="A9" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>76</v>
@@ -2815,21 +3749,21 @@
       </c>
       <c r="U9" s="31">
         <f>COUNTIF(H3:H90,"*Failed*")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="52">
       <c r="A10" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>102</v>
@@ -2858,21 +3792,21 @@
       </c>
       <c r="U10" s="31">
         <f>COUNTIF(H4:H90,"*Not*")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="76" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>103</v>
@@ -2890,7 +3824,7 @@
         <v>65</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>33</v>
@@ -2905,30 +3839,30 @@
         <v>83</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="65">
       <c r="A12" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="32" t="s">
         <v>134</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>135</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="36">
         <v>42086</v>
       </c>
       <c r="H12" s="26" t="s">
@@ -2937,9 +3871,7 @@
       <c r="I12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>136</v>
-      </c>
+      <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -2947,12 +3879,34 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:26">
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="10"/>
+    <row r="13" spans="1:26" ht="52">
+      <c r="A13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2961,26 +3915,82 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:26">
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+    <row r="14" spans="1:26" ht="65">
+      <c r="A14" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="K14" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="M14" s="34">
+        <v>42099</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:26">
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="10"/>
+    <row r="15" spans="1:26" ht="52">
+      <c r="A15" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2989,12 +3999,34 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:26">
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="10"/>
+    <row r="16" spans="1:26" ht="52">
+      <c r="A16" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -3003,11 +4035,31 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="5:21">
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
+    <row r="17" spans="1:21" ht="39">
+      <c r="A17" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>24</v>
+      </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -3017,11 +4069,31 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="5:21">
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
+    <row r="18" spans="1:21" ht="39">
+      <c r="A18" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>24</v>
+      </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -3031,11 +4103,31 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="5:21">
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="26"/>
+    <row r="19" spans="1:21" ht="39">
+      <c r="A19" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>24</v>
+      </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -3045,11 +4137,31 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="5:21">
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="26"/>
+    <row r="20" spans="1:21" ht="39">
+      <c r="A20" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>24</v>
+      </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -3059,11 +4171,31 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="5:21">
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="26"/>
+    <row r="21" spans="1:21" ht="52">
+      <c r="A21" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -3073,11 +4205,31 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="5:21">
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="26"/>
+    <row r="22" spans="1:21" ht="39">
+      <c r="A22" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -3087,11 +4239,31 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="5:21">
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="26"/>
+    <row r="23" spans="1:21" ht="52">
+      <c r="A23" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -3101,11 +4273,31 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="5:21">
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="26"/>
+    <row r="24" spans="1:21" ht="26">
+      <c r="A24" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -3115,11 +4307,31 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="5:21">
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="26"/>
+    <row r="25" spans="1:21" ht="26">
+      <c r="A25" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -3132,11 +4344,31 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="5:21">
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="26"/>
+    <row r="26" spans="1:21" ht="26">
+      <c r="A26" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -3150,14 +4382,34 @@
       </c>
       <c r="U26" s="31">
         <f>COUNTIF(L2:L50,"*Minor*")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="5:21">
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="26"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="26">
+      <c r="A27" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -3170,15 +4422,34 @@
         <v>57</v>
       </c>
       <c r="U27" s="31">
-        <f>COUNTIF(L2:L7,"*Moderate*")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="5:21">
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="26"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="26">
+      <c r="A28" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -3195,11 +4466,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:21">
-      <c r="E29" s="10"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="26"/>
+    <row r="29" spans="1:21" ht="39">
+      <c r="A29" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -3216,11 +4507,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="5:21">
-      <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="26"/>
+    <row r="30" spans="1:21" ht="26">
+      <c r="A30" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="36">
+        <v>42099</v>
+      </c>
+      <c r="H30" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -3237,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="5:21">
+    <row r="31" spans="1:21">
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="10"/>
@@ -3251,7 +4562,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="5:21">
+    <row r="32" spans="1:21">
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
@@ -5122,10 +6433,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF99FF99"/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5167,10 +6478,10 @@
     </row>
     <row r="2" spans="1:13" ht="42">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -5193,10 +6504,10 @@
     </row>
     <row r="3" spans="1:13" ht="56">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>78</v>
@@ -5218,10 +6529,10 @@
     </row>
     <row r="4" spans="1:13" ht="56">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>87</v>
@@ -5243,10 +6554,10 @@
     </row>
     <row r="5" spans="1:13" ht="42">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>87</v>
@@ -5268,10 +6579,10 @@
     </row>
     <row r="6" spans="1:13" ht="42">
       <c r="A6" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>100</v>
@@ -5293,10 +6604,10 @@
     </row>
     <row r="7" spans="1:13" ht="56">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>99</v>
@@ -5318,16 +6629,16 @@
     </row>
     <row r="8" spans="1:13" ht="56">
       <c r="A8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>68</v>
@@ -5343,16 +6654,16 @@
     </row>
     <row r="9" spans="1:13" ht="56">
       <c r="A9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>68</v>
@@ -5368,16 +6679,16 @@
     </row>
     <row r="10" spans="1:13" ht="56">
       <c r="A10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>68</v>
@@ -5393,16 +6704,16 @@
     </row>
     <row r="11" spans="1:13" ht="56">
       <c r="A11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>68</v>
@@ -5418,16 +6729,16 @@
     </row>
     <row r="12" spans="1:13" ht="71" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>68</v>
@@ -5441,12 +6752,22 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="1:13" ht="56">
+      <c r="A13" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -5456,12 +6777,22 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:13" ht="56">
+      <c r="A14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -5471,12 +6802,22 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:13" ht="42">
+      <c r="A15" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -5486,12 +6827,22 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="1:13" ht="42">
+      <c r="A16" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>208</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -5501,12 +6852,22 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+    <row r="17" spans="1:13" ht="28">
+      <c r="A17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>208</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -5516,12 +6877,22 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+    <row r="18" spans="1:13" ht="28">
+      <c r="A18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>208</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -5531,12 +6902,22 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+    <row r="19" spans="1:13" ht="28">
+      <c r="A19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>208</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -5545,6 +6926,193 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="28">
+      <c r="A20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="56">
+      <c r="A21" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28">
+      <c r="A22" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="56">
+      <c r="A23" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="28">
+      <c r="A24" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="28">
+      <c r="A25" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="28">
+      <c r="A26" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="28">
+      <c r="A27" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="28">
+      <c r="A28" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="28">
+      <c r="A29" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="28">
+      <c r="A30" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5649,6 +7217,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5762,22 +7345,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5791,21 +7376,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates and then changes to selenium
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
+++ b/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-760" yWindow="-460" windowWidth="25600" windowHeight="16000" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="309">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -430,9 +430,6 @@
     <t>automated selenium test</t>
   </si>
   <si>
-    <t>To test that the order receipt contains the items placed on order, specifically looking to see if it records the additional extras</t>
-  </si>
-  <si>
     <t>Have to have already placed an order and selected collection time to see the order receipt</t>
   </si>
   <si>
@@ -448,12 +445,6 @@
     <t>na</t>
   </si>
   <si>
-    <t>To test that the order receipt contains invididual prices for each item that have been ordered</t>
-  </si>
-  <si>
-    <t>Order receipt will show the total price for all items that have been ordered</t>
-  </si>
-  <si>
     <t>To test that the order receipt contains the total price for all items that have been ordered</t>
   </si>
   <si>
@@ -832,9 +823,6 @@
     <t>Having added an order to the basket with no extras and confirmed the collection time, take user to the order receipt. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
   </si>
   <si>
-    <t>Having added a plain cheese pizza to the basket with Olives, pepperoni, peppers and onions as extras and confirmed the collection time, take user to the order receipt. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
-  </si>
-  <si>
     <t>Having added an order to the basket with extras and confirmed the collection time, take user to the order receipt. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
   </si>
   <si>
@@ -976,9 +964,6 @@
     <t>There is a generic "unique" order reference used, though it is not critical, but the spec does suggest that the success of this business rests upon using a unique reference number, rendering it as a high priority defect. This case also fails on  the iPad4, the iPhone 6 and the Samsung Galaxy S4 mobile device as well as Firefox browser</t>
   </si>
   <si>
-    <t xml:space="preserve">To check for </t>
-  </si>
-  <si>
     <t>OrderReceipt_Tconn_14</t>
   </si>
   <si>
@@ -1018,9 +1003,6 @@
     <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Cheese pizza with Olives, Pepperoni, Peppers and Onions as extras</t>
   </si>
   <si>
-    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Meat Extravaganza with peppers and onions as extras and a Cheese pizza</t>
-  </si>
-  <si>
     <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with olives and a cheese pizza</t>
   </si>
   <si>
@@ -1043,6 +1025,144 @@
   </si>
   <si>
     <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:na</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TCase_26</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TCase_27</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic Deluxe pizza with Olives, Pepperoni, Peppers and Onions as extras</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza: Meat extravaganza pizza with Olives, Pepperoni, Peppers and Onions as extras</t>
+  </si>
+  <si>
+    <t>To test that the order receipt contains the items placed on order, specifically looking to see if it records the additional extras for specific pizza</t>
+  </si>
+  <si>
+    <t>To test that the order receipt contains the items placed on order, specifically looking to see if it records the additional extras  for specific pizza</t>
+  </si>
+  <si>
+    <t>Failed due to onions extra not being on the order receipt as well as incorrect price for meat extravaganza pizza on the order receipt. On further testing, this was apparent across all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_24</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_25</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_26</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_24</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_25</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_26</t>
+  </si>
+  <si>
+    <t>Having added a meat extravaganza pizza to the basket with Olives, pepperoni, peppers and onions as extras and confirmed the collection time, take user to the order receipt. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
+  </si>
+  <si>
+    <t>Having added a  classic deluxe pizza to the basket with Olives, pepperoni, peppers and onions as extras and confirmed the collection time, take user to the order receipt. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
+  </si>
+  <si>
+    <t>Having added a cheese pizza to the basket with Olives, pepperoni, peppers and onions as extras and confirmed the collection time, take user to the order receipt. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_27</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_27</t>
+  </si>
+  <si>
+    <t>To test the Orde Receipt page for general errors such as spelling mistakes</t>
+  </si>
+  <si>
+    <t>There will be little to no spelling mistakes on the order receipt page</t>
+  </si>
+  <si>
+    <t>To check for any spelling mistakes on the Order Receipt page</t>
+  </si>
+  <si>
+    <t>To test that the order receipt contains individual prices for each item that have been ordered</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with peppers and onions as extras and a Cheese pizza</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Meat extravaganza with olives and a cheese pizza</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TCase_28</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Meat extravaganza with onions and a cheese pizza</t>
+  </si>
+  <si>
+    <t>This failed as an incorrect price for the total was given. This failed across all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:2 x cheese pizza and 1 x classic deluxe</t>
+  </si>
+  <si>
+    <t>To test that the order receipt contains the total price for all items that have been ordered and that the price is correct</t>
+  </si>
+  <si>
+    <t>To test that the order receipt contains the total price for all items that have been ordered and that price is correct using different data</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TCase_29</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TCase_30</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_28</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_29</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_30</t>
+  </si>
+  <si>
+    <t>Order receipt will show a total price for the user's order</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_28</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_29</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_30</t>
+  </si>
+  <si>
+    <t>Order receipt will show a total price for the user's order and this price will be correct</t>
+  </si>
+  <si>
+    <t>Order receipt will show the total price for all items that have been ordered and this will be the correct price using different test data to that of the previous test</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with pepperoni           Later Date: 12 March 2015 @ 12:00</t>
+  </si>
+  <si>
+    <t>automated selenium test involving a manual intervention (note - for selenium, change the date and time on the value fields to the day you are testing in the same format as test has saved, this will enable the test to run successfully)</t>
+  </si>
+  <si>
+    <t>automated selenium test involving a manual intervention  (note - for selenium, change the date and time on the value fields to the day you are testing in the same format as test has saved, this will enable the test to run successfully)</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with pepperoni Later Date: 11 March 2015 @ 03:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with pepperoni Later Date: 10 March 2015 </t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1381,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="819">
+  <cellStyleXfs count="933">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2081,8 +2201,122 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2208,8 +2442,11 @@
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="819">
+  <cellStyles count="933">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2619,6 +2856,63 @@
     <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="914" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="916" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="918" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="920" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="922" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="924" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="926" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="928" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="930" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="932" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3028,6 +3322,63 @@
     <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="913" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="915" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="917" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="919" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="921" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="923" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="925" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="927" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="929" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="931" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -3144,10 +3495,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -3267,11 +3618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2122187048"/>
-        <c:axId val="2121896376"/>
+        <c:axId val="2090835112"/>
+        <c:axId val="2090838056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122187048"/>
+        <c:axId val="2090835112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3280,7 +3631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121896376"/>
+        <c:crossAx val="2090838056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3288,7 +3639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121896376"/>
+        <c:axId val="2090838056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3299,7 +3650,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122187048"/>
+        <c:crossAx val="2090835112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3739,13 +4090,13 @@
     </row>
     <row r="2" spans="1:9" ht="35.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -3756,13 +4107,13 @@
     </row>
     <row r="3" spans="1:9" ht="35.5" customHeight="1">
       <c r="A3" s="32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -3771,13 +4122,13 @@
     </row>
     <row r="4" spans="1:9" ht="28">
       <c r="A4" s="32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -3788,13 +4139,13 @@
     </row>
     <row r="5" spans="1:9" ht="23">
       <c r="A5" s="32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -3805,13 +4156,13 @@
     </row>
     <row r="6" spans="1:9" ht="28">
       <c r="A6" s="32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -3822,13 +4173,13 @@
     </row>
     <row r="7" spans="1:9" ht="28">
       <c r="A7" s="32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3839,13 +4190,13 @@
     </row>
     <row r="8" spans="1:9" ht="28">
       <c r="A8" s="32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3856,13 +4207,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -3870,13 +4221,13 @@
     </row>
     <row r="10" spans="1:9" ht="28">
       <c r="A10" s="32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -3884,13 +4235,13 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -3898,27 +4249,27 @@
     </row>
     <row r="12" spans="1:9" ht="28">
       <c r="A12" s="32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28">
       <c r="A13" s="32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -3926,13 +4277,13 @@
     </row>
     <row r="14" spans="1:9" ht="42">
       <c r="A14" s="32" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -3940,13 +4291,13 @@
     </row>
     <row r="15" spans="1:9" ht="42">
       <c r="A15" s="32" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -4207,8 +4558,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4280,19 +4631,19 @@
     </row>
     <row r="2" spans="1:26" ht="39">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -4319,19 +4670,19 @@
     </row>
     <row r="3" spans="1:26" ht="65">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>27</v>
@@ -4358,19 +4709,19 @@
     </row>
     <row r="4" spans="1:26" ht="65">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>267</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>27</v>
@@ -4395,21 +4746,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="52">
+    <row r="5" spans="1:26" ht="65">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>268</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>261</v>
+        <v>64</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>266</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>27</v>
@@ -4418,226 +4769,238 @@
         <v>42074</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
+      <c r="J5" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="33">
+        <v>42074</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>269</v>
+      </c>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:26" ht="52">
+    <row r="6" spans="1:26" ht="65">
       <c r="A6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>262</v>
+        <v>169</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>285</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="13">
+        <v>91</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="41">
         <v>42074</v>
       </c>
-      <c r="H6" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" s="33">
-        <v>42074</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>196</v>
-      </c>
+      <c r="J6" s="44"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="52">
       <c r="A7" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>263</v>
+        <v>170</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>286</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="13">
+        <v>91</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="41">
         <v>42074</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="44"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
       <c r="P7" s="10"/>
       <c r="T7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="39">
+    <row r="8" spans="1:26" ht="52">
       <c r="A8" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>263</v>
+        <v>171</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>290</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="13">
+        <v>92</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="41">
         <v>42074</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="44"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
       <c r="P8" s="10"/>
       <c r="T8" t="s">
         <v>53</v>
       </c>
       <c r="U8" s="31">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="52">
       <c r="A9" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>263</v>
+        <v>172</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>290</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="13">
+        <v>92</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="41">
         <v>42074</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="44"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
       <c r="P9" s="10"/>
       <c r="T9" t="s">
         <v>25</v>
       </c>
       <c r="U9" s="31">
         <f>COUNTIF(H3:H90,"*Failed*")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="52">
       <c r="A10" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>232</v>
+        <v>173</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>64</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="13">
+        <v>92</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="41">
         <v>42074</v>
       </c>
-      <c r="H10" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="12" t="s">
+      <c r="H10" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
+      <c r="J10" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="M10" s="47">
+        <v>42074</v>
+      </c>
+      <c r="N10" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="44" t="s">
+        <v>289</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="T10" t="s">
         <v>54</v>
@@ -4649,19 +5012,19 @@
     </row>
     <row r="11" spans="1:26" ht="76" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F11" s="40" t="s">
         <v>6</v>
@@ -4670,34 +5033,46 @@
         <v>42074</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I11" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
+      <c r="J11" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="47">
+        <v>42074</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>193</v>
+      </c>
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="52">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F12" s="40" t="s">
         <v>6</v>
@@ -4706,244 +5081,232 @@
         <v>42074</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="44" t="s">
-        <v>219</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>254</v>
-      </c>
-      <c r="M12" s="46">
-        <v>42074</v>
-      </c>
-      <c r="N12" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="45" t="s">
-        <v>245</v>
-      </c>
+      <c r="J12" s="44"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="52">
       <c r="A13" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>90</v>
+        <v>191</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F13" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="39">
-        <v>42086</v>
+      <c r="G13" s="41">
+        <v>42074</v>
       </c>
       <c r="H13" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="45" t="s">
+      <c r="I13" s="43" t="s">
         <v>62</v>
       </c>
       <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
+      <c r="K13" s="4"/>
       <c r="L13" s="45"/>
       <c r="M13" s="45"/>
       <c r="N13" s="45"/>
       <c r="O13" s="45"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:26" ht="39">
+    <row r="14" spans="1:26" ht="52">
       <c r="A14" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>120</v>
+        <v>192</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>267</v>
+        <v>307</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="39">
-        <v>42099</v>
+        <v>6</v>
+      </c>
+      <c r="G14" s="41">
+        <v>42074</v>
       </c>
       <c r="H14" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="43" t="s">
         <v>62</v>
       </c>
       <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
+      <c r="K14" s="4"/>
       <c r="L14" s="45"/>
       <c r="M14" s="45"/>
       <c r="N14" s="45"/>
       <c r="O14" s="45"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:26" ht="39">
+    <row r="15" spans="1:26" ht="52">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>121</v>
+        <v>228</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>109</v>
+        <v>229</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="39">
-        <v>42099</v>
+        <v>6</v>
+      </c>
+      <c r="G15" s="41">
+        <v>42074</v>
       </c>
       <c r="H15" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="M15" s="46">
-        <v>42099</v>
-      </c>
-      <c r="N15" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="O15" s="32" t="s">
-        <v>230</v>
-      </c>
+      <c r="J15" s="45"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
       <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="39">
       <c r="A16" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="39">
-        <v>42099</v>
+        <v>6</v>
+      </c>
+      <c r="G16" s="41">
+        <v>42074</v>
       </c>
       <c r="H16" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="45" t="s">
+      <c r="I16" s="43" t="s">
         <v>62</v>
       </c>
       <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
+      <c r="K16" s="4"/>
       <c r="L16" s="45"/>
       <c r="M16" s="45"/>
       <c r="N16" s="45"/>
       <c r="O16" s="45"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:21" ht="39">
+    <row r="17" spans="1:21" ht="52">
       <c r="A17" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F17" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="39">
-        <v>42099</v>
+        <v>6</v>
+      </c>
+      <c r="G17" s="41">
+        <v>42074</v>
       </c>
       <c r="H17" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
+      <c r="J17" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="M17" s="46">
+        <v>42074</v>
+      </c>
+      <c r="N17" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="45" t="s">
+        <v>241</v>
+      </c>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:21" ht="39">
+    <row r="18" spans="1:21" ht="52">
       <c r="A18" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="F18" s="40" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G18" s="39">
-        <v>42099</v>
+        <v>42086</v>
       </c>
       <c r="H18" s="42" t="s">
         <v>24</v>
@@ -4961,19 +5324,19 @@
     </row>
     <row r="19" spans="1:21" ht="39">
       <c r="A19" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F19" s="40" t="s">
         <v>11</v>
@@ -4997,19 +5360,19 @@
     </row>
     <row r="20" spans="1:21" ht="39">
       <c r="A20" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F20" s="40" t="s">
         <v>11</v>
@@ -5018,34 +5381,46 @@
         <v>42099</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I20" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="J20" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="M20" s="46">
+        <v>42099</v>
+      </c>
+      <c r="N20" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="32" t="s">
+        <v>226</v>
+      </c>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="1:21" ht="52">
+    <row r="21" spans="1:21" ht="39">
       <c r="A21" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F21" s="40" t="s">
         <v>11</v>
@@ -5069,19 +5444,19 @@
     </row>
     <row r="22" spans="1:21" ht="39">
       <c r="A22" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F22" s="40" t="s">
         <v>11</v>
@@ -5105,70 +5480,58 @@
     </row>
     <row r="23" spans="1:21" ht="39">
       <c r="A23" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G23" s="39">
         <v>42099</v>
       </c>
       <c r="H23" s="42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="45" t="s">
-        <v>221</v>
-      </c>
-      <c r="K23" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="L23" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="M23" s="46">
-        <v>42099</v>
-      </c>
-      <c r="N23" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="O23" s="45" t="s">
-        <v>255</v>
-      </c>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
       <c r="P23" s="10"/>
     </row>
     <row r="24" spans="1:21" ht="39">
       <c r="A24" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G24" s="39">
         <v>42099</v>
@@ -5181,7 +5544,7 @@
       </c>
       <c r="J24" s="45"/>
       <c r="K24" s="45"/>
-      <c r="L24" s="35"/>
+      <c r="L24" s="45"/>
       <c r="M24" s="45"/>
       <c r="N24" s="45"/>
       <c r="O24" s="45"/>
@@ -5189,89 +5552,77 @@
     </row>
     <row r="25" spans="1:21" ht="39">
       <c r="A25" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>268</v>
+        <v>244</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>261</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="36">
+      <c r="G25" s="39">
         <v>42099</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H25" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
       <c r="P25" s="10"/>
       <c r="T25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="39">
+    <row r="26" spans="1:21" ht="52">
       <c r="A26" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>268</v>
+        <v>245</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>255</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="F26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="10" t="s">
+      <c r="G26" s="39">
+        <v>42099</v>
+      </c>
+      <c r="H26" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="J26" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="K26" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="L26" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="M26" s="34">
-        <v>42099</v>
-      </c>
-      <c r="N26" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="O26" s="10" t="s">
-        <v>253</v>
-      </c>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="45"/>
       <c r="P26" s="10"/>
       <c r="T26" t="s">
         <v>34</v>
@@ -5281,22 +5632,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
+    <row r="27" spans="1:21" ht="39">
+      <c r="A27" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="39">
+        <v>42099</v>
+      </c>
+      <c r="H27" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="45"/>
       <c r="P27" s="10"/>
       <c r="T27" t="s">
         <v>57</v>
@@ -5305,22 +5674,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="1"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="1"/>
+    <row r="28" spans="1:21" ht="39">
+      <c r="A28" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="39">
+        <v>42099</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="M28" s="46">
+        <v>42099</v>
+      </c>
+      <c r="N28" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="O28" s="45" t="s">
+        <v>250</v>
+      </c>
       <c r="P28" s="10"/>
       <c r="T28" t="s">
         <v>35</v>
@@ -5329,22 +5728,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
+    <row r="29" spans="1:21" ht="39">
+      <c r="A29" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="39">
+        <v>42099</v>
+      </c>
+      <c r="H29" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
       <c r="P29" s="10"/>
       <c r="T29" t="s">
         <v>36</v>
@@ -5354,22 +5771,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
+    <row r="30" spans="1:21" ht="39">
+      <c r="A30" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="39">
+        <v>42099</v>
+      </c>
+      <c r="H30" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="35"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
       <c r="P30" s="10"/>
       <c r="T30" t="s">
         <v>38</v>
@@ -5378,22 +5813,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="1"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
+    <row r="31" spans="1:21" ht="39">
+      <c r="A31" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J31" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M31" s="46">
+        <v>42099</v>
+      </c>
+      <c r="N31" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="O31" s="45" t="s">
+        <v>248</v>
+      </c>
       <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:21">
@@ -7321,25 +7786,25 @@
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H10 H25:H53</xm:sqref>
+          <xm:sqref>H2:H5 H32:H53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F10 F25:F159</xm:sqref>
+          <xm:sqref>F2:F5 F32:F159</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L7</xm:sqref>
+          <xm:sqref>L2:L5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K10</xm:sqref>
+          <xm:sqref>K2:K5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7357,8 +7822,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7400,19 +7865,19 @@
     </row>
     <row r="2" spans="1:13" ht="98">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="27" t="s">
@@ -7426,19 +7891,19 @@
     </row>
     <row r="3" spans="1:13" ht="112">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>198</v>
+        <v>278</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -7449,21 +7914,21 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="98">
+    <row r="4" spans="1:13" ht="112">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>199</v>
+        <v>277</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -7474,21 +7939,21 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="98">
+    <row r="5" spans="1:13" ht="126">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>199</v>
+        <v>276</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -7501,19 +7966,19 @@
     </row>
     <row r="6" spans="1:13" ht="98">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>256</v>
+        <v>104</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>251</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -7524,21 +7989,21 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="112">
+    <row r="7" spans="1:13" ht="98">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>256</v>
+        <v>105</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>251</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -7549,21 +8014,21 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="112">
+    <row r="8" spans="1:13" ht="98">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>256</v>
+        <v>106</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>251</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -7574,21 +8039,21 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="112">
+    <row r="9" spans="1:13" ht="98">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>256</v>
+        <v>107</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>251</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -7599,21 +8064,21 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="126">
+    <row r="10" spans="1:13" ht="98">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>256</v>
+        <v>108</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>251</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -7624,21 +8089,21 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="112">
-      <c r="A11" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>111</v>
+    <row r="11" spans="1:13" ht="126">
+      <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>256</v>
+        <v>305</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -7650,20 +8115,20 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="71" customHeight="1">
-      <c r="A12" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>112</v>
+      <c r="A12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>257</v>
+        <v>306</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -7674,21 +8139,21 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="98">
-      <c r="A13" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>113</v>
+    <row r="13" spans="1:13" ht="126">
+      <c r="A13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>256</v>
+        <v>306</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -7699,21 +8164,21 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="98">
-      <c r="A14" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>129</v>
+    <row r="14" spans="1:13" ht="126">
+      <c r="A14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>134</v>
+        <v>306</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -7724,21 +8189,21 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="112">
-      <c r="A15" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>130</v>
+    <row r="15" spans="1:13" ht="126">
+      <c r="A15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -7749,21 +8214,21 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="98">
-      <c r="A16" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>131</v>
+    <row r="16" spans="1:13" ht="112">
+      <c r="A16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -7774,21 +8239,21 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="98">
-      <c r="A17" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>132</v>
+    <row r="17" spans="1:13" ht="112">
+      <c r="A17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>134</v>
+        <v>252</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -7799,21 +8264,21 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="84">
-      <c r="A18" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>143</v>
+    <row r="18" spans="1:13" ht="98">
+      <c r="A18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -7824,21 +8289,21 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="84">
-      <c r="A19" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>144</v>
+    <row r="19" spans="1:13" ht="98">
+      <c r="A19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -7849,155 +8314,215 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="84">
-      <c r="A20" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B20" s="32" t="s">
+    <row r="20" spans="1:13" ht="112">
+      <c r="A20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="98">
+      <c r="A21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="98">
+      <c r="A22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="84">
+      <c r="A23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="84">
+      <c r="A24" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="E24" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="84">
+      <c r="A25" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="84">
+      <c r="A26" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="78">
+      <c r="A27" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="91">
+      <c r="A28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="91">
+      <c r="A29" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="84">
-      <c r="A21" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="78">
-      <c r="A22" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="32" t="s">
+      <c r="D29" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="C22" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="91">
-      <c r="A23" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="E23" s="32" t="s">
+      <c r="E29" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="91">
-      <c r="A24" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="56">
-      <c r="A25" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="32"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="32"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="32"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="32"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="32"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="32"/>
+    <row r="30" spans="1:13" ht="56">
+      <c r="A30" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="42">
+      <c r="A31" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="32"/>
     </row>
     <row r="33" spans="1:5">
@@ -8250,6 +8775,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -8363,22 +8903,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8392,21 +8934,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
forgot the spreadsheet, my bad
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
+++ b/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-760" yWindow="-460" windowWidth="25600" windowHeight="16000" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="660" yWindow="280" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="310">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -1012,9 +1012,6 @@
     <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with pepperoni</t>
   </si>
   <si>
-    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic Deluxe with olives</t>
-  </si>
-  <si>
     <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Meat Extravaganza</t>
   </si>
   <si>
@@ -1163,6 +1160,12 @@
   </si>
   <si>
     <t xml:space="preserve">Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic deluxe with pepperoni Later Date: 10 March 2015 </t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                  Pizza:Classic Deluxe with olives   Later Date: 10 March 2015 @ 03:00</t>
+  </si>
+  <si>
+    <t>Login: ahale03@qub.ac.uk    Password :lespaul260                         New Password: adamhale03               Pizza:Classic Deluxe with olives</t>
   </si>
 </sst>
 </file>
@@ -4558,8 +4561,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4673,7 +4676,7 @@
         <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>64</v>
@@ -4712,13 +4715,13 @@
         <v>167</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>91</v>
@@ -4751,13 +4754,13 @@
         <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>91</v>
@@ -4790,7 +4793,7 @@
         <v>68</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P5" s="10"/>
     </row>
@@ -4799,13 +4802,13 @@
         <v>169</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E6" s="32" t="s">
         <v>91</v>
@@ -4835,13 +4838,13 @@
         <v>170</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E7" s="32" t="s">
         <v>91</v>
@@ -4880,7 +4883,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>92</v>
@@ -4917,13 +4920,13 @@
         <v>172</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>92</v>
@@ -4960,13 +4963,13 @@
         <v>173</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>92</v>
@@ -4999,7 +5002,7 @@
         <v>68</v>
       </c>
       <c r="O10" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P10" s="10"/>
       <c r="T10" t="s">
@@ -5069,7 +5072,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>102</v>
@@ -5105,7 +5108,7 @@
         <v>64</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>102</v>
@@ -5141,7 +5144,7 @@
         <v>64</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>102</v>
@@ -5177,7 +5180,7 @@
         <v>228</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>229</v>
@@ -5213,7 +5216,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>103</v>
@@ -5249,7 +5252,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>103</v>
@@ -5297,7 +5300,7 @@
         <v>88</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>104</v>
@@ -5333,7 +5336,7 @@
         <v>118</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>105</v>
@@ -5369,7 +5372,7 @@
         <v>118</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>106</v>
@@ -5453,7 +5456,7 @@
         <v>118</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>108</v>
@@ -5525,7 +5528,7 @@
         <v>118</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E24" s="32" t="s">
         <v>108</v>
@@ -5561,7 +5564,7 @@
         <v>118</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E25" s="32" t="s">
         <v>108</v>
@@ -5634,7 +5637,7 @@
     </row>
     <row r="27" spans="1:21" ht="39">
       <c r="A27" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>152</v>
@@ -5643,7 +5646,7 @@
         <v>118</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>109</v>
@@ -5676,7 +5679,7 @@
     </row>
     <row r="28" spans="1:21" ht="39">
       <c r="A28" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>153</v>
@@ -5685,7 +5688,7 @@
         <v>118</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>110</v>
@@ -5730,7 +5733,7 @@
     </row>
     <row r="29" spans="1:21" ht="39">
       <c r="A29" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>154</v>
@@ -5739,7 +5742,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>126</v>
@@ -5773,7 +5776,7 @@
     </row>
     <row r="30" spans="1:21" ht="39">
       <c r="A30" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>231</v>
@@ -5782,7 +5785,7 @@
         <v>68</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E30" s="32" t="s">
         <v>127</v>
@@ -5815,16 +5818,16 @@
     </row>
     <row r="31" spans="1:21" ht="39">
       <c r="A31" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>242</v>
@@ -7822,8 +7825,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A24" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7897,7 +7900,7 @@
         <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>66</v>
@@ -7922,7 +7925,7 @@
         <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>66</v>
@@ -7947,7 +7950,7 @@
         <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>66</v>
@@ -8025,7 +8028,7 @@
         <v>195</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>251</v>
@@ -8050,7 +8053,7 @@
         <v>195</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>251</v>
@@ -8075,7 +8078,7 @@
         <v>195</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>251</v>
@@ -8103,7 +8106,7 @@
         <v>70</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -8128,7 +8131,7 @@
         <v>70</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -8153,7 +8156,7 @@
         <v>73</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -8178,7 +8181,7 @@
         <v>73</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -8401,10 +8404,10 @@
     </row>
     <row r="25" spans="1:13" ht="84">
       <c r="A25" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C25" s="32" t="s">
         <v>209</v>
@@ -8418,10 +8421,10 @@
     </row>
     <row r="26" spans="1:13" ht="84">
       <c r="A26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>210</v>
@@ -8435,10 +8438,10 @@
     </row>
     <row r="27" spans="1:13" ht="78">
       <c r="A27" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="38" t="s">
         <v>211</v>
@@ -8452,10 +8455,10 @@
     </row>
     <row r="28" spans="1:13" ht="91">
       <c r="A28" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="C28" s="38" t="s">
         <v>212</v>
@@ -8469,10 +8472,10 @@
     </row>
     <row r="29" spans="1:13" ht="91">
       <c r="A29" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C29" s="38" t="s">
         <v>213</v>
@@ -8486,10 +8489,10 @@
     </row>
     <row r="30" spans="1:13" ht="56">
       <c r="A30" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C30" s="32" t="s">
         <v>239</v>
@@ -8503,16 +8506,16 @@
     </row>
     <row r="31" spans="1:13" ht="42">
       <c r="A31" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C31" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D31" s="32" t="s">
         <v>281</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>282</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
small change for changing graphs
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
+++ b/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="0" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="314">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -703,9 +703,6 @@
     <t>Any user that is not registered should not be able to access the Order Receipt page</t>
   </si>
   <si>
-    <t>To ensure all logged users can navigate to the reset password page</t>
-  </si>
-  <si>
     <t>To check that unregistered users or not logged in users can't access the Order Receipt page</t>
   </si>
   <si>
@@ -892,9 +889,6 @@
     <t>OrderReceipt_4</t>
   </si>
   <si>
-    <t>4.1.6, 3.2.1, 3.2.2</t>
-  </si>
-  <si>
     <t>4.1.10, 3.2.2</t>
   </si>
   <si>
@@ -1175,6 +1169,15 @@
   </si>
   <si>
     <t>Manual Test</t>
+  </si>
+  <si>
+    <t>To ensure all logged users can navigate to the reset password page and should be able to log out from the order receipt page</t>
+  </si>
+  <si>
+    <t>4.1.6, 4.1.9, 3.2.1, 3.2.2</t>
+  </si>
+  <si>
+    <t>automated selenium test and manual test for mavigation to forgot password page</t>
   </si>
 </sst>
 </file>
@@ -3456,7 +3459,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3466,7 +3468,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3476,7 +3477,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3541,7 +3541,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3638,11 +3637,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2065458120"/>
-        <c:axId val="2065461064"/>
+        <c:axId val="2091673432"/>
+        <c:axId val="2091676376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2065458120"/>
+        <c:axId val="2091673432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3651,7 +3650,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065461064"/>
+        <c:crossAx val="2091676376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3659,7 +3658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2065461064"/>
+        <c:axId val="2091676376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3670,7 +3669,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065458120"/>
+        <c:crossAx val="2091673432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4084,7 +4083,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4116,7 +4115,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -4133,7 +4132,7 @@
         <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -4145,10 +4144,10 @@
         <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4165,7 +4164,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -4179,10 +4178,10 @@
         <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -4199,7 +4198,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -4216,7 +4215,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4233,7 +4232,7 @@
         <v>114</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4247,7 +4246,7 @@
         <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4258,24 +4257,24 @@
         <v>100</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28">
+    <row r="12" spans="1:9" ht="42">
       <c r="A12" s="32" t="s">
         <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>311</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>116</v>
@@ -4286,10 +4285,10 @@
         <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>218</v>
+        <v>312</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -4297,13 +4296,13 @@
     </row>
     <row r="14" spans="1:9" ht="42">
       <c r="A14" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -4311,13 +4310,13 @@
     </row>
     <row r="15" spans="1:9" ht="42">
       <c r="A15" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -4578,8 +4577,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4651,7 +4650,7 @@
     </row>
     <row r="2" spans="1:26" ht="39">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
@@ -4660,7 +4659,7 @@
         <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>91</v>
@@ -4690,16 +4689,16 @@
     </row>
     <row r="3" spans="1:26" ht="65">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>91</v>
@@ -4729,16 +4728,16 @@
     </row>
     <row r="4" spans="1:26" ht="65">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>91</v>
@@ -4768,16 +4767,16 @@
     </row>
     <row r="5" spans="1:26" ht="65">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>91</v>
@@ -4795,7 +4794,7 @@
         <v>62</v>
       </c>
       <c r="J5" s="44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>33</v>
@@ -4810,22 +4809,22 @@
         <v>68</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:26" ht="65">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E6" s="32" t="s">
         <v>91</v>
@@ -4852,16 +4851,16 @@
     </row>
     <row r="7" spans="1:26" ht="52">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E7" s="32" t="s">
         <v>91</v>
@@ -4891,7 +4890,7 @@
     </row>
     <row r="8" spans="1:26" ht="52">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>69</v>
@@ -4900,7 +4899,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>92</v>
@@ -4934,16 +4933,16 @@
     </row>
     <row r="9" spans="1:26" ht="52">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>92</v>
@@ -4977,16 +4976,16 @@
     </row>
     <row r="10" spans="1:26" ht="52">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>92</v>
@@ -5004,13 +5003,13 @@
         <v>62</v>
       </c>
       <c r="J10" s="44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M10" s="47">
         <v>42074</v>
@@ -5019,7 +5018,7 @@
         <v>68</v>
       </c>
       <c r="O10" s="44" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="P10" s="10"/>
       <c r="T10" t="s">
@@ -5032,7 +5031,7 @@
     </row>
     <row r="11" spans="1:26" ht="76" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>71</v>
@@ -5041,7 +5040,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>102</v>
@@ -5059,7 +5058,7 @@
         <v>62</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>33</v>
@@ -5074,13 +5073,13 @@
         <v>68</v>
       </c>
       <c r="O11" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="52">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>72</v>
@@ -5089,7 +5088,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>102</v>
@@ -5116,16 +5115,16 @@
     </row>
     <row r="13" spans="1:26" ht="52">
       <c r="A13" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>102</v>
@@ -5152,16 +5151,16 @@
     </row>
     <row r="14" spans="1:26" ht="52">
       <c r="A14" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>102</v>
@@ -5188,19 +5187,19 @@
     </row>
     <row r="15" spans="1:26" ht="52">
       <c r="A15" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>227</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>229</v>
       </c>
       <c r="F15" s="40" t="s">
         <v>6</v>
@@ -5224,7 +5223,7 @@
     </row>
     <row r="16" spans="1:26" ht="39">
       <c r="A16" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>86</v>
@@ -5233,7 +5232,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>103</v>
@@ -5260,7 +5259,7 @@
     </row>
     <row r="17" spans="1:21" ht="52">
       <c r="A17" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>85</v>
@@ -5269,7 +5268,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>103</v>
@@ -5287,7 +5286,7 @@
         <v>62</v>
       </c>
       <c r="J17" s="44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>33</v>
@@ -5302,13 +5301,13 @@
         <v>68</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:21" ht="52">
       <c r="A18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>87</v>
@@ -5317,7 +5316,7 @@
         <v>88</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>104</v>
@@ -5344,7 +5343,7 @@
     </row>
     <row r="19" spans="1:21" ht="39">
       <c r="A19" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>117</v>
@@ -5353,7 +5352,7 @@
         <v>118</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>105</v>
@@ -5380,7 +5379,7 @@
     </row>
     <row r="20" spans="1:21" ht="39">
       <c r="A20" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>119</v>
@@ -5389,7 +5388,7 @@
         <v>118</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>106</v>
@@ -5407,7 +5406,7 @@
         <v>62</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K20" s="35" t="s">
         <v>33</v>
@@ -5422,13 +5421,13 @@
         <v>68</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:21" ht="39">
       <c r="A21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>120</v>
@@ -5437,7 +5436,7 @@
         <v>118</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E21" s="32" t="s">
         <v>107</v>
@@ -5464,7 +5463,7 @@
     </row>
     <row r="22" spans="1:21" ht="39">
       <c r="A22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>121</v>
@@ -5473,7 +5472,7 @@
         <v>118</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>108</v>
@@ -5500,7 +5499,7 @@
     </row>
     <row r="23" spans="1:21" ht="39">
       <c r="A23" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>149</v>
@@ -5509,7 +5508,7 @@
         <v>118</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>140</v>
@@ -5536,7 +5535,7 @@
     </row>
     <row r="24" spans="1:21" ht="39">
       <c r="A24" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>148</v>
@@ -5545,7 +5544,7 @@
         <v>118</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E24" s="32" t="s">
         <v>108</v>
@@ -5572,7 +5571,7 @@
     </row>
     <row r="25" spans="1:21" ht="39">
       <c r="A25" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>150</v>
@@ -5581,7 +5580,7 @@
         <v>118</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E25" s="32" t="s">
         <v>108</v>
@@ -5611,7 +5610,7 @@
     </row>
     <row r="26" spans="1:21" ht="52">
       <c r="A26" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B26" s="38" t="s">
         <v>151</v>
@@ -5620,7 +5619,7 @@
         <v>118</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E26" s="32" t="s">
         <v>108</v>
@@ -5654,7 +5653,7 @@
     </row>
     <row r="27" spans="1:21" ht="39">
       <c r="A27" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>152</v>
@@ -5663,7 +5662,7 @@
         <v>118</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>109</v>
@@ -5696,7 +5695,7 @@
     </row>
     <row r="28" spans="1:21" ht="39">
       <c r="A28" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>153</v>
@@ -5705,7 +5704,7 @@
         <v>118</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>110</v>
@@ -5723,7 +5722,7 @@
         <v>62</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="K28" s="35" t="s">
         <v>33</v>
@@ -5738,7 +5737,7 @@
         <v>68</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="P28" s="10"/>
       <c r="T28" t="s">
@@ -5750,7 +5749,7 @@
     </row>
     <row r="29" spans="1:21" ht="39">
       <c r="A29" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>154</v>
@@ -5759,7 +5758,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>126</v>
@@ -5792,16 +5791,16 @@
     </row>
     <row r="30" spans="1:21" ht="39">
       <c r="A30" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E30" s="32" t="s">
         <v>127</v>
@@ -5834,25 +5833,25 @@
     </row>
     <row r="31" spans="1:21" ht="39">
       <c r="A31" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F31" s="40" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H31" s="42" t="s">
         <v>25</v>
@@ -5861,7 +5860,7 @@
         <v>62</v>
       </c>
       <c r="J31" s="45" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K31" s="35" t="s">
         <v>33</v>
@@ -5876,7 +5875,7 @@
         <v>68</v>
       </c>
       <c r="O31" s="45" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="P31" s="10"/>
     </row>
@@ -7841,8 +7840,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7890,13 +7889,13 @@
         <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="27" t="s">
@@ -7916,13 +7915,13 @@
         <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -7941,13 +7940,13 @@
         <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -7966,13 +7965,13 @@
         <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -7991,13 +7990,13 @@
         <v>104</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -8016,13 +8015,13 @@
         <v>105</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -8041,13 +8040,13 @@
         <v>106</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -8066,13 +8065,13 @@
         <v>107</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -8091,13 +8090,13 @@
         <v>108</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -8116,13 +8115,13 @@
         <v>109</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>70</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -8141,13 +8140,13 @@
         <v>110</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D12" s="32" t="s">
         <v>70</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -8166,13 +8165,13 @@
         <v>126</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -8191,13 +8190,13 @@
         <v>127</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>73</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -8216,13 +8215,13 @@
         <v>128</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -8241,13 +8240,13 @@
         <v>129</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>82</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -8266,13 +8265,13 @@
         <v>140</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D17" s="32" t="s">
         <v>82</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -8291,13 +8290,13 @@
         <v>141</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>90</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -8316,13 +8315,13 @@
         <v>142</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>130</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -8341,146 +8340,146 @@
         <v>143</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D20" s="32" t="s">
         <v>132</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="98">
       <c r="A21" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" s="32" t="s">
         <v>133</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="98">
       <c r="A22" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>134</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="84">
       <c r="A23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>144</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="84">
       <c r="A24" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>145</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="84">
       <c r="A25" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>146</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="84">
       <c r="A26" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>147</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="78">
       <c r="A27" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="91">
       <c r="A28" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>63</v>
@@ -8488,33 +8487,33 @@
     </row>
     <row r="29" spans="1:13" ht="91">
       <c r="A29" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>63</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="56">
       <c r="A30" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E30" s="32" t="s">
         <v>131</v>
@@ -8522,16 +8521,16 @@
     </row>
     <row r="31" spans="1:13" ht="42">
       <c r="A31" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>131</v>
@@ -8794,6 +8793,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -8907,22 +8921,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8936,21 +8952,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final changes i hope
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
+++ b/Testing Spreadsheet v1.0 OrderReceipt_AdamHale.xlsx
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="320">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -871,9 +871,6 @@
     <t>From the Order Receipt page, a logged user can navigate to the reset password page. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. This will be a manual / exploratory test.</t>
   </si>
   <si>
-    <t>A logged user should be able to log off from the Order Receipt page. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
-  </si>
-  <si>
     <t>The system should prevent unregistered users accessing the Schedule Order page. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
   </si>
   <si>
@@ -976,9 +973,6 @@
     <t>Where it says "you're logged in as &lt;username&gt;, it is highlighten in bold with a full stop at the end. This could be confusing as having the full stop in bold may lead some users to think they have input their email incorrect. This is extremely minor and fussy however, but is consistent across all browsers and mobile devices</t>
   </si>
   <si>
-    <t>Major</t>
-  </si>
-  <si>
     <t xml:space="preserve">When clicking on the log out button, the user is first redirected to the Order Page. They are not directly logged out straight away, it is only when this is clicked for a second time is the user logged out. This fails across all the browsers  as well as all the mobile devices listed in the spec </t>
   </si>
   <si>
@@ -1178,6 +1172,30 @@
   </si>
   <si>
     <t>automated selenium test and manual test for mavigation to forgot password page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any user can navigate to the forgot password page by clicking on their email address on the top right of the wedsite </t>
+  </si>
+  <si>
+    <t>be logged in and on the order receipt page</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TCase_31</t>
+  </si>
+  <si>
+    <t>Users are able to get to the reset password page</t>
+  </si>
+  <si>
+    <t>A logged in user should be able to log off from the Order Receipt page. This will be tested across all mobile devices that have been listed in the spec, as well as all the browsers. The automated test shall be made and recorded through Firefox browser</t>
+  </si>
+  <si>
+    <t>A logged in user should be able to navigate to the Forgot password page while on the Order Receipt page</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TProc_31</t>
+  </si>
+  <si>
+    <t>OrderReceipt_TConn_31</t>
   </si>
 </sst>
 </file>
@@ -1396,8 +1414,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="937">
+  <cellStyleXfs count="957">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2465,7 +2503,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="937">
+  <cellStyles count="957">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2934,6 +2972,16 @@
     <cellStyle name="Followed Hyperlink" xfId="932" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="934" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="936" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="938" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="948" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="950" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="952" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="954" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="956" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3402,6 +3450,16 @@
     <cellStyle name="Hyperlink" xfId="931" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="933" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="935" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="937" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="947" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="949" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="951" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="953" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="955" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -3459,6 +3517,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3468,6 +3527,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3477,6 +3537,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3515,7 +3576,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7.0</c:v>
@@ -3541,6 +3602,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3613,13 +3675,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.0</c:v>
@@ -3637,11 +3699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2091673432"/>
-        <c:axId val="2091676376"/>
+        <c:axId val="2097851256"/>
+        <c:axId val="2097854200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091673432"/>
+        <c:axId val="2097851256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3650,7 +3712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091676376"/>
+        <c:crossAx val="2097854200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3658,7 +3720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091676376"/>
+        <c:axId val="2097854200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3669,7 +3731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091673432"/>
+        <c:crossAx val="2097851256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4115,7 +4177,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -4132,7 +4194,7 @@
         <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -4147,7 +4209,7 @@
         <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4164,7 +4226,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -4181,7 +4243,7 @@
         <v>188</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -4198,7 +4260,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -4215,7 +4277,7 @@
         <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4232,7 +4294,7 @@
         <v>114</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4246,7 +4308,7 @@
         <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4260,7 +4322,7 @@
         <v>189</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4271,10 +4333,10 @@
         <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>116</v>
@@ -4288,7 +4350,7 @@
         <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -4296,13 +4358,13 @@
     </row>
     <row r="14" spans="1:9" ht="42">
       <c r="A14" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="C14" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -4310,13 +4372,13 @@
     </row>
     <row r="15" spans="1:9" ht="42">
       <c r="A15" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>240</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -4577,8 +4639,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A27" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4659,7 +4721,7 @@
         <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>91</v>
@@ -4692,13 +4754,13 @@
         <v>165</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>91</v>
@@ -4731,13 +4793,13 @@
         <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>91</v>
@@ -4770,13 +4832,13 @@
         <v>167</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>91</v>
@@ -4794,13 +4856,13 @@
         <v>62</v>
       </c>
       <c r="J5" s="44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="M5" s="33">
         <v>42074</v>
@@ -4809,7 +4871,7 @@
         <v>68</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P5" s="10"/>
     </row>
@@ -4818,13 +4880,13 @@
         <v>168</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E6" s="32" t="s">
         <v>91</v>
@@ -4854,13 +4916,13 @@
         <v>169</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E7" s="32" t="s">
         <v>91</v>
@@ -4899,7 +4961,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>92</v>
@@ -4928,7 +4990,7 @@
       </c>
       <c r="U8" s="31">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="52">
@@ -4936,13 +4998,13 @@
         <v>171</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>92</v>
@@ -4979,13 +5041,13 @@
         <v>172</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>92</v>
@@ -5003,13 +5065,13 @@
         <v>62</v>
       </c>
       <c r="J10" s="44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>246</v>
+        <v>57</v>
       </c>
       <c r="M10" s="47">
         <v>42074</v>
@@ -5018,7 +5080,7 @@
         <v>68</v>
       </c>
       <c r="O10" s="44" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="P10" s="10"/>
       <c r="T10" t="s">
@@ -5040,7 +5102,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>102</v>
@@ -5058,7 +5120,7 @@
         <v>62</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>33</v>
@@ -5088,7 +5150,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>102</v>
@@ -5124,7 +5186,7 @@
         <v>64</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>102</v>
@@ -5160,7 +5222,7 @@
         <v>64</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>102</v>
@@ -5190,16 +5252,16 @@
         <v>177</v>
       </c>
       <c r="B15" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="D15" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>226</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>305</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>227</v>
       </c>
       <c r="F15" s="40" t="s">
         <v>6</v>
@@ -5232,7 +5294,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>103</v>
@@ -5268,7 +5330,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>103</v>
@@ -5286,13 +5348,13 @@
         <v>62</v>
       </c>
       <c r="J17" s="44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="35" t="s">
-        <v>36</v>
+      <c r="L17" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="M17" s="46">
         <v>42074</v>
@@ -5301,7 +5363,7 @@
         <v>68</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P17" s="10"/>
     </row>
@@ -5316,7 +5378,7 @@
         <v>88</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>104</v>
@@ -5352,7 +5414,7 @@
         <v>118</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>105</v>
@@ -5388,7 +5450,7 @@
         <v>118</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>106</v>
@@ -5406,7 +5468,7 @@
         <v>62</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K20" s="35" t="s">
         <v>33</v>
@@ -5421,7 +5483,7 @@
         <v>68</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P20" s="10"/>
     </row>
@@ -5436,7 +5498,7 @@
         <v>118</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E21" s="32" t="s">
         <v>107</v>
@@ -5472,7 +5534,7 @@
         <v>118</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>108</v>
@@ -5508,7 +5570,7 @@
         <v>118</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>140</v>
@@ -5535,7 +5597,7 @@
     </row>
     <row r="24" spans="1:21" ht="39">
       <c r="A24" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>148</v>
@@ -5544,7 +5606,7 @@
         <v>118</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E24" s="32" t="s">
         <v>108</v>
@@ -5571,7 +5633,7 @@
     </row>
     <row r="25" spans="1:21" ht="39">
       <c r="A25" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>150</v>
@@ -5580,7 +5642,7 @@
         <v>118</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E25" s="32" t="s">
         <v>108</v>
@@ -5610,7 +5672,7 @@
     </row>
     <row r="26" spans="1:21" ht="52">
       <c r="A26" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B26" s="38" t="s">
         <v>151</v>
@@ -5619,7 +5681,7 @@
         <v>118</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E26" s="32" t="s">
         <v>108</v>
@@ -5653,7 +5715,7 @@
     </row>
     <row r="27" spans="1:21" ht="39">
       <c r="A27" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>152</v>
@@ -5662,7 +5724,7 @@
         <v>118</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>109</v>
@@ -5690,12 +5752,12 @@
         <v>57</v>
       </c>
       <c r="U27" s="31">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="39">
       <c r="A28" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>153</v>
@@ -5704,7 +5766,7 @@
         <v>118</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>110</v>
@@ -5722,7 +5784,7 @@
         <v>62</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K28" s="35" t="s">
         <v>33</v>
@@ -5737,19 +5799,19 @@
         <v>68</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="P28" s="10"/>
       <c r="T28" t="s">
         <v>35</v>
       </c>
       <c r="U28" s="31">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="39">
       <c r="A29" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>154</v>
@@ -5758,7 +5820,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>126</v>
@@ -5786,27 +5848,27 @@
         <v>36</v>
       </c>
       <c r="U29" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="52">
       <c r="A30" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>229</v>
+        <v>312</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>68</v>
+        <v>313</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="G30" s="39">
         <v>42099</v>
@@ -5833,68 +5895,86 @@
     </row>
     <row r="31" spans="1:21" ht="39">
       <c r="A31" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>239</v>
+        <v>127</v>
       </c>
       <c r="F31" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="39" t="s">
-        <v>243</v>
+      <c r="G31" s="39">
+        <v>42099</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="J31" s="45" t="s">
-        <v>308</v>
-      </c>
-      <c r="K31" s="35" t="s">
+      <c r="J31" s="35"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:21" ht="39">
+      <c r="A32" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J32" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="K32" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="L31" s="35" t="s">
+      <c r="L32" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="M31" s="46">
+      <c r="M32" s="46">
         <v>42099</v>
       </c>
-      <c r="N31" s="45" t="s">
+      <c r="N32" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="O31" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="P31" s="10"/>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
+      <c r="O32" s="45" t="s">
+        <v>244</v>
+      </c>
       <c r="P32" s="10"/>
     </row>
     <row r="33" spans="1:16">
@@ -7804,19 +7884,19 @@
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H5 H32:H53</xm:sqref>
+          <xm:sqref>H2:H5 H33:H53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F5 F32:F159</xm:sqref>
+          <xm:sqref>F2:F5 F33:F159</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L5</xm:sqref>
+          <xm:sqref>L2:L5 L10 L17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -7840,8 +7920,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7895,7 +7975,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="27" t="s">
@@ -7915,13 +7995,13 @@
         <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -7940,13 +8020,13 @@
         <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -7965,13 +8045,13 @@
         <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -7996,7 +8076,7 @@
         <v>67</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -8021,7 +8101,7 @@
         <v>67</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -8043,10 +8123,10 @@
         <v>194</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -8068,10 +8148,10 @@
         <v>194</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -8093,10 +8173,10 @@
         <v>194</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -8121,7 +8201,7 @@
         <v>70</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -8146,7 +8226,7 @@
         <v>70</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -8171,7 +8251,7 @@
         <v>73</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -8196,7 +8276,7 @@
         <v>73</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -8215,13 +8295,13 @@
         <v>128</v>
       </c>
       <c r="C15" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>234</v>
-      </c>
       <c r="E15" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -8246,7 +8326,7 @@
         <v>82</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -8271,7 +8351,7 @@
         <v>82</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -8296,7 +8376,7 @@
         <v>90</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -8321,7 +8401,7 @@
         <v>130</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -8346,7 +8426,7 @@
         <v>132</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="98">
@@ -8363,7 +8443,7 @@
         <v>133</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="98">
@@ -8380,7 +8460,7 @@
         <v>134</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="84">
@@ -8397,15 +8477,15 @@
         <v>144</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="84">
       <c r="A24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>207</v>
@@ -8414,15 +8494,15 @@
         <v>145</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="84">
       <c r="A25" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C25" s="32" t="s">
         <v>208</v>
@@ -8431,15 +8511,15 @@
         <v>146</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="84">
       <c r="A26" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>209</v>
@@ -8448,15 +8528,15 @@
         <v>147</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="78">
       <c r="A27" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C27" s="38" t="s">
         <v>210</v>
@@ -8465,18 +8545,18 @@
         <v>163</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="91">
       <c r="A28" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>211</v>
+        <v>316</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>186</v>
@@ -8487,61 +8567,71 @@
     </row>
     <row r="29" spans="1:13" ht="91">
       <c r="A29" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>162</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="56">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="42">
       <c r="A30" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C30" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="56">
+      <c r="A31" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>238</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="42">
-      <c r="A31" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>278</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="1"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
+    <row r="32" spans="1:13" ht="42">
+      <c r="A32" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
@@ -8793,21 +8883,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -8921,15 +9002,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8938,7 +9020,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8952,4 +9034,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>